<commit_message>
refactor and created func to store database
</commit_message>
<xml_diff>
--- a/phishing-acciones.xlsx
+++ b/phishing-acciones.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\INSUMOS\fbarreto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B630FD6-8CA2-4C76-88B7-AC61E2943224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE187C6-C32E-45AD-95C3-9E847154CE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{9194A3E8-E572-4B93-9A0D-697364509B27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{9194A3E8-E572-4B93-9A0D-697364509B27}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$1:$E$17</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
   <si>
     <t>PROCESO</t>
   </si>
@@ -157,12 +160,6 @@
   </si>
   <si>
     <t>irodri@bcp.gov.py</t>
-  </si>
-  <si>
-    <t>Ultimo aviso pre - Judicial  - AAREM-264967241</t>
-  </si>
-  <si>
-    <t>Ultimo aviso pre - Judicial  - AAREM-264967242</t>
   </si>
   <si>
     <t>Ultimo aviso pre - Judicial  - AAREM-264967243</t>
@@ -193,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,7 +255,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -560,7 +557,7 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
@@ -568,7 +565,7 @@
     <col min="4" max="4" width="46.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -582,7 +579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -596,7 +593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -610,7 +607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -621,7 +618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -639,13 +636,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D4F454-7D89-467E-9E69-0402D3EF1B22}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
@@ -654,7 +651,7 @@
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -671,7 +668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -688,7 +685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -705,7 +702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -722,7 +719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -739,7 +736,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -756,7 +753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -773,7 +770,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -790,7 +787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -807,7 +804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -824,7 +821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -841,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -858,7 +855,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -875,15 +872,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1">
-        <v>45231</v>
+        <v>45243</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -892,15 +889,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1">
-        <v>45231</v>
+        <v>45243</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -909,12 +906,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1">
         <v>45243</v>
@@ -926,12 +923,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1">
         <v>45243</v>
@@ -943,41 +940,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="1">
-        <v>45243</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="1">
-        <v>45243</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:E17" xr:uid="{99D4F454-7D89-467E-9E69-0402D3EF1B22}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>